<commit_message>
Completed reconfiguration tests and recorded results
</commit_message>
<xml_diff>
--- a/Reconfig-Experiments/Results/ReconfigurationExperiments.xlsx
+++ b/Reconfig-Experiments/Results/ReconfigurationExperiments.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20935927\Documents\Masters-Case-Study\Reconfig-Experiments\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE19ED3-68D5-448B-B919-C6AA43E4246C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C78910-5621-471D-A18A-A7B181BDC749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment_1" sheetId="1" r:id="rId1"/>
-    <sheet name="Experiment_2" sheetId="2" r:id="rId2"/>
-    <sheet name="Experiemnt_3" sheetId="3" r:id="rId3"/>
+    <sheet name="Experiement_2" sheetId="3" r:id="rId2"/>
+    <sheet name="Experiment_3" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="39">
   <si>
     <t>Description:</t>
   </si>
@@ -129,6 +129,30 @@
   </si>
   <si>
     <t>Mention complexity of electricity pricing in South Africa so an average amount will be used: R1.209</t>
+  </si>
+  <si>
+    <t>SpawnOnMap.cs</t>
+  </si>
+  <si>
+    <t>Adding total energy usage service to DTs (gives the total energy usage reading for a given period)</t>
+  </si>
+  <si>
+    <t>Adding total energy usage service to conv (gives the total energy usage reading for a given period)</t>
+  </si>
+  <si>
+    <t>EnergyCostService.cs</t>
+  </si>
+  <si>
+    <t>ServiceGateway.cs</t>
+  </si>
+  <si>
+    <t>ServerSocket.cs</t>
+  </si>
+  <si>
+    <t>Bootstrap.cs</t>
+  </si>
+  <si>
+    <t>ConfigurationFile</t>
   </si>
 </sst>
 </file>
@@ -170,12 +194,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,7 +481,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:O23"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,349 +837,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA3B8638-9121-4684-A529-585405CEBDCF}">
-  <dimension ref="A1:S23"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="L2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2">
-        <v>697</v>
-      </c>
-      <c r="N2">
-        <v>881</v>
-      </c>
-      <c r="O2">
-        <f>N2-M2</f>
-        <v>184</v>
-      </c>
-      <c r="S2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M3">
-        <v>27</v>
-      </c>
-      <c r="N3">
-        <v>29</v>
-      </c>
-      <c r="O3">
-        <f t="shared" ref="O3:O10" si="0">N3-M3</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="L4" t="s">
-        <v>15</v>
-      </c>
-      <c r="M4">
-        <v>33</v>
-      </c>
-      <c r="N4">
-        <v>35</v>
-      </c>
-      <c r="O4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="R4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="L5" t="s">
-        <v>16</v>
-      </c>
-      <c r="M5">
-        <v>123</v>
-      </c>
-      <c r="N5">
-        <v>138</v>
-      </c>
-      <c r="O5">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-      <c r="L6" t="s">
-        <v>17</v>
-      </c>
-      <c r="M6">
-        <v>636</v>
-      </c>
-      <c r="N6">
-        <v>819</v>
-      </c>
-      <c r="O6">
-        <f t="shared" si="0"/>
-        <v>183</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="L7" t="s">
-        <v>18</v>
-      </c>
-      <c r="M7">
-        <v>1023</v>
-      </c>
-      <c r="N7">
-        <v>1310</v>
-      </c>
-      <c r="O7">
-        <f t="shared" si="0"/>
-        <v>287</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="L8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M8">
-        <v>68</v>
-      </c>
-      <c r="N8">
-        <v>76</v>
-      </c>
-      <c r="O8">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
-      <c r="L9" t="s">
-        <v>16</v>
-      </c>
-      <c r="M9">
-        <v>68</v>
-      </c>
-      <c r="N9">
-        <v>76</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="L10" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10">
-        <v>413</v>
-      </c>
-      <c r="N10">
-        <v>422</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="O11">
-        <f>SUM(O2:O10)</f>
-        <v>698</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-      <c r="L15" t="s">
-        <v>9</v>
-      </c>
-      <c r="M15" t="s">
-        <v>10</v>
-      </c>
-      <c r="N15" t="s">
-        <v>11</v>
-      </c>
-      <c r="O15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="L16" t="s">
-        <v>23</v>
-      </c>
-      <c r="M16">
-        <v>694</v>
-      </c>
-      <c r="N16">
-        <v>953</v>
-      </c>
-      <c r="O16">
-        <f>N16-M16</f>
-        <v>259</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>2</v>
-      </c>
-      <c r="L17" t="s">
-        <v>24</v>
-      </c>
-      <c r="M17">
-        <v>170</v>
-      </c>
-      <c r="N17">
-        <v>308</v>
-      </c>
-      <c r="O17">
-        <f t="shared" ref="O17:O18" si="1">N17-M17</f>
-        <v>138</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="L18" t="s">
-        <v>19</v>
-      </c>
-      <c r="M18">
-        <v>709</v>
-      </c>
-      <c r="N18">
-        <v>718</v>
-      </c>
-      <c r="O18">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O19">
-        <f>SUM(O16:O18)</f>
-        <v>406</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="4"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD270277-57A0-4EF2-8822-31D6A11004EC}">
   <dimension ref="A1:O23"/>
   <sheetViews>
@@ -1172,7 +851,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="L1" t="s">
         <v>9</v>
@@ -1192,14 +871,14 @@
         <v>13</v>
       </c>
       <c r="M2">
-        <v>697</v>
+        <v>883</v>
       </c>
       <c r="N2">
-        <v>881</v>
+        <v>992</v>
       </c>
       <c r="O2">
         <f>N2-M2</f>
-        <v>184</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1210,14 +889,14 @@
         <v>14</v>
       </c>
       <c r="M3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="N3">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O10" si="0">N3-M3</f>
-        <v>2</v>
+        <f t="shared" ref="O3:O7" si="0">N3-M3</f>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1225,35 +904,35 @@
         <v>20</v>
       </c>
       <c r="B4" s="1">
-        <v>0.11458333333333333</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="L4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="M4">
-        <v>33</v>
+        <v>819</v>
       </c>
       <c r="N4">
-        <v>35</v>
+        <v>1023</v>
       </c>
       <c r="O4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M5">
-        <v>123</v>
+        <v>1310</v>
       </c>
       <c r="N5">
-        <v>138</v>
+        <v>1599</v>
       </c>
       <c r="O5">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>289</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1276,65 +955,56 @@
         <v>21</v>
       </c>
       <c r="L6" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="M6">
-        <v>636</v>
+        <v>191</v>
       </c>
       <c r="N6">
-        <v>819</v>
+        <v>195</v>
       </c>
       <c r="O6">
         <f t="shared" si="0"/>
-        <v>183</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
-        <f>O10</f>
-        <v>9</v>
+        <f>O6+O7</f>
+        <v>8</v>
       </c>
       <c r="C7" s="2">
         <v>0</v>
       </c>
       <c r="D7" s="2">
-        <f>SUM(O2:O9)</f>
-        <v>689</v>
+        <f>SUM(O2:O5)</f>
+        <v>605</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
       </c>
       <c r="F7" s="2">
         <f>SUM(B7:E7)</f>
-        <v>698</v>
+        <v>613</v>
       </c>
       <c r="L7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M7">
-        <v>1023</v>
+        <v>422</v>
       </c>
       <c r="N7">
-        <v>1310</v>
+        <v>426</v>
       </c>
       <c r="O7">
         <f t="shared" si="0"/>
-        <v>287</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M8">
-        <v>68</v>
-      </c>
-      <c r="N8">
-        <v>76</v>
-      </c>
       <c r="O8">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f>SUM(O2:O7)</f>
+        <v>613</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1353,47 +1023,13 @@
       <c r="E9" t="s">
         <v>7</v>
       </c>
-      <c r="L9" t="s">
-        <v>16</v>
-      </c>
-      <c r="M9">
-        <v>68</v>
-      </c>
-      <c r="N9">
-        <v>76</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L10" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10">
-        <v>413</v>
-      </c>
-      <c r="N10">
-        <v>422</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O11">
-        <f>SUM(O2:O10)</f>
-        <v>698</v>
-      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="L15" t="s">
         <v>9</v>
@@ -1413,10 +1049,10 @@
         <v>23</v>
       </c>
       <c r="M16">
-        <v>694</v>
+        <v>953</v>
       </c>
       <c r="N16">
-        <v>953</v>
+        <v>1212</v>
       </c>
       <c r="O16">
         <f>N16-M16</f>
@@ -1431,14 +1067,14 @@
         <v>24</v>
       </c>
       <c r="M17">
-        <v>170</v>
+        <v>308</v>
       </c>
       <c r="N17">
-        <v>308</v>
+        <v>437</v>
       </c>
       <c r="O17">
         <f t="shared" ref="O17:O18" si="1">N17-M17</f>
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -1446,26 +1082,374 @@
         <v>20</v>
       </c>
       <c r="B18" s="1">
-        <v>1.4583333333333332E-2</v>
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="L18" t="s">
+        <v>31</v>
+      </c>
+      <c r="M18">
+        <v>184</v>
+      </c>
+      <c r="N18">
+        <v>188</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>19</v>
+      </c>
+      <c r="M19">
+        <v>718</v>
+      </c>
+      <c r="N19">
+        <v>722</v>
+      </c>
+      <c r="O19">
+        <f>N19-M19</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="O20">
+        <f>SUM(O16:O19)</f>
+        <v>396</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <f>O20</f>
+        <v>396</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA3B8638-9121-4684-A529-585405CEBDCF}">
+  <dimension ref="A1:S23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>84</v>
+      </c>
+      <c r="O2">
+        <f>N2-M2</f>
+        <v>84</v>
+      </c>
+      <c r="S2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3">
+        <v>74</v>
+      </c>
+      <c r="N3">
+        <v>86</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O8" si="0">N3-M3</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="L4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4">
+        <v>127</v>
+      </c>
+      <c r="N4">
+        <v>133</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="R4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5">
+        <v>21</v>
+      </c>
+      <c r="N5">
+        <v>24</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6">
+        <v>195</v>
+      </c>
+      <c r="N6">
+        <v>199</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <f>O6+O7</f>
+        <v>17</v>
+      </c>
+      <c r="C7" s="2">
+        <f>SUM(O2:O5)</f>
+        <v>105</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <f>O8</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <f>SUM(B7:E7)</f>
+        <v>123</v>
+      </c>
+      <c r="L7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7">
+        <v>426</v>
+      </c>
+      <c r="N7">
+        <v>439</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8">
+        <v>4</v>
+      </c>
+      <c r="N8">
+        <v>5</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="O9">
+        <f>SUM(O2:O8)</f>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="L15" t="s">
+        <v>9</v>
+      </c>
+      <c r="M15" t="s">
+        <v>10</v>
+      </c>
+      <c r="N15" t="s">
+        <v>11</v>
+      </c>
+      <c r="O15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L16" t="s">
+        <v>23</v>
+      </c>
+      <c r="M16">
+        <v>1214</v>
+      </c>
+      <c r="N16">
+        <v>1257</v>
+      </c>
+      <c r="O16">
+        <f>N16-M16</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="L17" t="s">
+        <v>31</v>
+      </c>
+      <c r="M17">
+        <v>188</v>
+      </c>
+      <c r="N17">
+        <v>192</v>
+      </c>
+      <c r="O17">
+        <f t="shared" ref="O17" si="1">N17-M17</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1">
+        <v>8.3333333333333332E-3</v>
       </c>
       <c r="L18" t="s">
         <v>19</v>
       </c>
       <c r="M18">
-        <v>709</v>
+        <v>722</v>
       </c>
       <c r="N18">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="O18">
-        <f t="shared" si="1"/>
-        <v>9</v>
+        <f>N18-M18</f>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="O19">
         <f>SUM(O16:O18)</f>
-        <v>406</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1479,7 +1463,7 @@
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <f>O19</f>
-        <v>406</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Processed reconfiguration test results.
Calculated reused code percentage for all 3 reconfig experiments and recorded them in the Results excel file.
</commit_message>
<xml_diff>
--- a/Reconfig-Experiments/Results/ReconfigurationExperiments.xlsx
+++ b/Reconfig-Experiments/Results/ReconfigurationExperiments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20935927\Documents\Masters-Case-Study\Reconfig-Experiments\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Masters-Case-Study\Reconfig-Experiments\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C78910-5621-471D-A18A-A7B181BDC749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7EF492-B369-44A4-A45B-ACA739530EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment_1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="47">
   <si>
     <t>Description:</t>
   </si>
@@ -153,6 +153,30 @@
   </si>
   <si>
     <t>ConfigurationFile</t>
+  </si>
+  <si>
+    <t>Percentage Code Reused</t>
+  </si>
+  <si>
+    <t>Total Code Reused</t>
+  </si>
+  <si>
+    <t>Lines Reused</t>
+  </si>
+  <si>
+    <t>Completely new lines</t>
+  </si>
+  <si>
+    <t>Source Code</t>
+  </si>
+  <si>
+    <t>Total Lines Added</t>
+  </si>
+  <si>
+    <t>PrecinctDBDataAccess.cs</t>
+  </si>
+  <si>
+    <t>CampusDBDataAccess.cs</t>
   </si>
 </sst>
 </file>
@@ -478,28 +502,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.109375" customWidth="1"/>
+    <col min="12" max="12" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -518,8 +544,14 @@
       <c r="O1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L2" t="s">
         <v>13</v>
       </c>
@@ -533,8 +565,16 @@
         <f>N2-M2</f>
         <v>184</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2">
+        <f>O2-Q2</f>
+        <v>114</v>
+      </c>
+      <c r="Q2">
+        <f>39+15+9+3+4</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -542,17 +582,23 @@
         <v>14</v>
       </c>
       <c r="M3">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N3">
         <v>29</v>
       </c>
       <c r="O3">
         <f t="shared" ref="O3:O10" si="0">N3-M3</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -572,8 +618,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L5" t="s">
         <v>16</v>
       </c>
@@ -587,8 +639,15 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5">
+        <f>O5-Q5</f>
+        <v>2</v>
+      </c>
+      <c r="Q5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -620,8 +679,16 @@
         <f t="shared" si="0"/>
         <v>183</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6">
+        <f>51+9+63+17</f>
+        <v>140</v>
+      </c>
+      <c r="Q6">
+        <f>O6-P6</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <f>O10</f>
         <v>9</v>
@@ -631,14 +698,14 @@
       </c>
       <c r="D7" s="2">
         <f>SUM(O2:O9)</f>
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
       </c>
       <c r="F7" s="2">
         <f>SUM(B7:E7)</f>
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="L7" t="s">
         <v>18</v>
@@ -653,10 +720,18 @@
         <f t="shared" si="0"/>
         <v>287</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7">
+        <f>O7-Q7</f>
+        <v>211</v>
+      </c>
+      <c r="Q7">
+        <f>3+3+33+12+12+9+4</f>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L8" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="M8">
         <v>68</v>
@@ -668,8 +743,15 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8">
+        <f>O8-Q8</f>
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -685,8 +767,11 @@
       <c r="E9" t="s">
         <v>7</v>
       </c>
+      <c r="F9" t="s">
+        <v>40</v>
+      </c>
       <c r="L9" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="M9">
         <v>68</v>
@@ -698,8 +783,33 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9">
+        <f>O9-Q9</f>
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B10" s="2">
+        <f>P10</f>
+        <v>6</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <f>SUM(P2:P9)</f>
+        <v>469</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <f>SUM(B10:E10)</f>
+        <v>475</v>
+      </c>
       <c r="L10" t="s">
         <v>19</v>
       </c>
@@ -713,14 +823,70 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10">
+        <f>O10-Q10</f>
+        <v>6</v>
+      </c>
+      <c r="Q10">
+        <f>2+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="O11">
         <f>SUM(O2:O10)</f>
-        <v>698</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+        <v>699</v>
+      </c>
+      <c r="P11">
+        <f t="shared" ref="P11:Q11" si="1">SUM(P2:P10)</f>
+        <v>475</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="1"/>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B13" s="2">
+        <f>(B10/B7)*100</f>
+        <v>66.666666666666657</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <f>(D10/D7)*100</f>
+        <v>67.971014492753625</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <f>(F10/F7)*100</f>
+        <v>67.954220314735338</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -739,8 +905,14 @@
       <c r="O15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P15" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L16" t="s">
         <v>23</v>
       </c>
@@ -754,8 +926,16 @@
         <f>N16-M16</f>
         <v>259</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P16">
+        <f>O16-Q16</f>
+        <v>226</v>
+      </c>
+      <c r="Q16">
+        <f>5+14+14</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -769,11 +949,19 @@
         <v>308</v>
       </c>
       <c r="O17">
-        <f t="shared" ref="O17:O18" si="1">N17-M17</f>
+        <f t="shared" ref="O17:O18" si="2">N17-M17</f>
         <v>138</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P17">
+        <f>O17-Q17</f>
+        <v>109</v>
+      </c>
+      <c r="Q17">
+        <f>5+24</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -790,45 +978,111 @@
         <v>718</v>
       </c>
       <c r="O18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P18">
+        <f>O18-Q18</f>
+        <v>6</v>
+      </c>
+      <c r="Q18">
+        <f>3</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="O19">
         <f>SUM(O16:O18)</f>
         <v>406</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P19">
+        <f>SUM(P16:P18)</f>
+        <v>341</v>
+      </c>
+      <c r="Q19">
+        <f>SUM(Q16:Q18)</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B21" s="2">
         <f>O19</f>
         <v>406</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2">
+        <f>SUM(B21:C21)</f>
+        <v>406</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B24" s="2">
+        <f>P19</f>
+        <v>341</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2">
+        <f>SUM(B24:C24)</f>
+        <v>341</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" t="s">
         <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B27" s="2">
+        <f>(B24/B21)*100</f>
+        <v>83.990147783251231</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" ref="C27:D27" si="3">(D24/D21)*100</f>
+        <v>83.990147783251231</v>
       </c>
     </row>
   </sheetData>
@@ -838,15 +1092,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD270277-57A0-4EF2-8822-31D6A11004EC}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:O23"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -865,8 +1130,14 @@
       <c r="O1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L2" t="s">
         <v>13</v>
       </c>
@@ -880,8 +1151,16 @@
         <f>N2-M2</f>
         <v>109</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2">
+        <f>O2-Q2</f>
+        <v>56</v>
+      </c>
+      <c r="Q2">
+        <f>6+15+15+9+4+4</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -898,8 +1177,15 @@
         <f t="shared" ref="O3:O7" si="0">N3-M3</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3">
+        <f>O3-Q3</f>
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -919,8 +1205,16 @@
         <f t="shared" si="0"/>
         <v>204</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4">
+        <f t="shared" ref="P4:P7" si="1">O4-Q4</f>
+        <v>169</v>
+      </c>
+      <c r="Q4">
+        <f>25+10</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L5" t="s">
         <v>18</v>
       </c>
@@ -934,8 +1228,16 @@
         <f t="shared" si="0"/>
         <v>289</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>207</v>
+      </c>
+      <c r="Q5">
+        <f>3+19+27+16+9+8</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -967,8 +1269,15 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="Q6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <f>O6+O7</f>
         <v>8</v>
@@ -1000,14 +1309,29 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="Q7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="O8">
         <f>SUM(O2:O7)</f>
         <v>613</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8">
+        <f>SUM(P2:P7)</f>
+        <v>436</v>
+      </c>
+      <c r="Q8">
+        <f>SUM(Q2:Q7)</f>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1023,8 +1347,71 @@
       <c r="E9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B10" s="2">
+        <f>P7+P6</f>
+        <v>4</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <f>SUM(P2:P5)</f>
+        <v>432</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <f>SUM(B10:E10)</f>
+        <v>436</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B13" s="2">
+        <f>(B10/B7)*100</f>
+        <v>50</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <f>(D10/D7)*100</f>
+        <v>71.404958677685954</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <f>(F10/F7)*100</f>
+        <v>71.125611745513865</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1043,8 +1430,14 @@
       <c r="O15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P15" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L16" t="s">
         <v>23</v>
       </c>
@@ -1058,8 +1451,16 @@
         <f>N16-M16</f>
         <v>259</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P16">
+        <f>O16-Q16</f>
+        <v>224</v>
+      </c>
+      <c r="Q16">
+        <f>9+17+9</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1073,11 +1474,19 @@
         <v>437</v>
       </c>
       <c r="O17">
-        <f t="shared" ref="O17:O18" si="1">N17-M17</f>
+        <f t="shared" ref="O17:O18" si="2">N17-M17</f>
         <v>129</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P17">
+        <f>O17-Q17</f>
+        <v>107</v>
+      </c>
+      <c r="Q17">
+        <f>5+17</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1094,11 +1503,18 @@
         <v>188</v>
       </c>
       <c r="O18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P18">
+        <f>O18-Q18</f>
+        <v>2</v>
+      </c>
+      <c r="Q18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L19" t="s">
         <v>19</v>
       </c>
@@ -1112,40 +1528,105 @@
         <f>N19-M19</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P19">
+        <f>O19-Q19</f>
+        <v>2</v>
+      </c>
+      <c r="Q19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>44</v>
       </c>
       <c r="O20">
         <f>SUM(O16:O19)</f>
         <v>396</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P20">
+        <f>SUM(P16:P19)</f>
+        <v>335</v>
+      </c>
+      <c r="Q20">
+        <f>SUM(Q16:Q18)</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B21" s="2">
         <f>O20</f>
         <v>396</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2">
+        <f>SUM(B21:C21)</f>
+        <v>396</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B24" s="2">
+        <f>P20</f>
+        <v>335</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2">
+        <f>SUM(B24:C24)</f>
+        <v>335</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" t="s">
         <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B27" s="2">
+        <f>(B24/B21)*100</f>
+        <v>84.595959595959584</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" ref="D27" si="3">(D24/D21)*100</f>
+        <v>84.595959595959584</v>
       </c>
     </row>
   </sheetData>
@@ -1155,20 +1636,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA3B8638-9121-4684-A529-585405CEBDCF}">
-  <dimension ref="A1:S23"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.21875" customWidth="1"/>
+    <col min="13" max="13" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1187,14 +1678,14 @@
       <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="R1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L2" t="s">
         <v>34</v>
       </c>
@@ -1208,11 +1699,15 @@
         <f>N2-M2</f>
         <v>84</v>
       </c>
-      <c r="S2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P2">
+        <f>O2-Q2</f>
+        <v>69</v>
+      </c>
+      <c r="Q2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1229,8 +1724,15 @@
         <f t="shared" ref="O3:O8" si="0">N3-M3</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P3">
+        <f>O3-Q3</f>
+        <v>10</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1250,11 +1752,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="R4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P4">
+        <f t="shared" ref="P4:P8" si="1">O4-Q4</f>
+        <v>2</v>
+      </c>
+      <c r="Q4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L5" t="s">
         <v>37</v>
       </c>
@@ -1268,8 +1774,15 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1301,8 +1814,15 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="Q6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <f>O6+O7</f>
         <v>17</v>
@@ -1335,8 +1855,15 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P7">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="Q7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L8" t="s">
         <v>38</v>
       </c>
@@ -1350,8 +1877,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1366,13 +1900,84 @@
       </c>
       <c r="E9" t="s">
         <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>40</v>
       </c>
       <c r="O9">
         <f>SUM(O2:O8)</f>
         <v>123</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P9">
+        <f>SUM(P2:P8)</f>
+        <v>87</v>
+      </c>
+      <c r="Q9">
+        <f>SUM(Q2:Q8)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B10" s="2">
+        <f>P7+P6</f>
+        <v>6</v>
+      </c>
+      <c r="C10" s="2">
+        <f>SUM(P2:P5)</f>
+        <v>81</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <f>P8</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <f>SUM(B10:E10)</f>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B13" s="2">
+        <f>(B10/B7)*100</f>
+        <v>35.294117647058826</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <f>(F10/F7)*100</f>
+        <v>70.731707317073173</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1391,8 +1996,14 @@
       <c r="O15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P15" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L16" t="s">
         <v>23</v>
       </c>
@@ -1406,8 +2017,15 @@
         <f>N16-M16</f>
         <v>43</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P16">
+        <f>O16-Q16</f>
+        <v>30</v>
+      </c>
+      <c r="Q16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1421,11 +2039,18 @@
         <v>192</v>
       </c>
       <c r="O17">
-        <f t="shared" ref="O17" si="1">N17-M17</f>
+        <f t="shared" ref="O17" si="2">N17-M17</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P17">
+        <f>O17-Q17</f>
+        <v>2</v>
+      </c>
+      <c r="Q17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1445,42 +2070,121 @@
         <f>N18-M18</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P18">
+        <f>O18-Q18</f>
+        <v>2</v>
+      </c>
+      <c r="Q18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="O19">
         <f>SUM(O16:O18)</f>
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P19">
+        <f t="shared" ref="P19:Q19" si="3">SUM(P16:P18)</f>
+        <v>34</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B21" s="2">
         <f>O19</f>
         <v>51</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2">
+        <f>SUM(B21:C21)</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B24" s="2">
+        <f>P19</f>
+        <v>34</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2">
+        <f>SUM(B24:C24)</f>
+        <v>34</v>
+      </c>
+      <c r="L24" t="s">
+        <v>27</v>
+      </c>
+      <c r="M24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="M25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" t="s">
         <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B27" s="2">
+        <f>(B24/B21)*100</f>
+        <v>66.666666666666657</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" ref="D27" si="4">(D24/D21)*100</f>
+        <v>66.666666666666657</v>
+      </c>
+      <c r="L27" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Processing of evaluation results
</commit_message>
<xml_diff>
--- a/Reconfig-Experiments/Results/ReconfigurationExperiments.xlsx
+++ b/Reconfig-Experiments/Results/ReconfigurationExperiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Masters-Case-Study\Reconfig-Experiments\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7EF492-B369-44A4-A45B-ACA739530EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988A8D8C-A80A-4AA9-9697-1607B59BA8D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment_1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="53">
   <si>
     <t>Description:</t>
   </si>
@@ -177,6 +177,24 @@
   </si>
   <si>
     <t>CampusDBDataAccess.cs</t>
+  </si>
+  <si>
+    <t>Unity code (%)</t>
+  </si>
+  <si>
+    <t>Services Code (%)</t>
+  </si>
+  <si>
+    <t>DT code (%)</t>
+  </si>
+  <si>
+    <t>Configuration File (%)</t>
+  </si>
+  <si>
+    <t>Percentage Code Reused (%)</t>
+  </si>
+  <si>
+    <t>Source Code (%)</t>
   </si>
 </sst>
 </file>
@@ -504,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -851,19 +869,19 @@
         <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
@@ -1063,13 +1081,13 @@
         <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="D26" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
@@ -1081,7 +1099,7 @@
         <v>0</v>
       </c>
       <c r="D27" s="2">
-        <f t="shared" ref="C27:D27" si="3">(D24/D21)*100</f>
+        <f t="shared" ref="D27" si="3">(D24/D21)*100</f>
         <v>83.990147783251231</v>
       </c>
     </row>
@@ -1095,7 +1113,7 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1376,19 +1394,19 @@
         <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
@@ -1607,13 +1625,13 @@
         <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="D26" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
@@ -1638,8 +1656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA3B8638-9121-4684-A529-585405CEBDCF}">
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1943,19 +1961,19 @@
         <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
@@ -2162,13 +2180,13 @@
         <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="D26" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>